<commit_message>
Updated User stories (#14, #3)
</commit_message>
<xml_diff>
--- a/documentation/User_stories Your Pizza App.xlsx
+++ b/documentation/User_stories Your Pizza App.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idris\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Silver\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{16904AFF-B430-4E35-823B-5BA136CF5118}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7292B729-7DA2-446E-8246-EBDB427F256D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Klant" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>Als</t>
   </si>
@@ -100,12 +100,6 @@
     <t>Een gedetailleerde overzicht van de samengestelde pizza die besteld is.</t>
   </si>
   <si>
-    <t>Keukenvoorraad kunnen inzien aanpassen en beheren.</t>
-  </si>
-  <si>
-    <t>Klant bevestiging sturen wanneer de bestelling is ontvangen.</t>
-  </si>
-  <si>
     <t>Klant</t>
   </si>
   <si>
@@ -118,30 +112,15 @@
     <t>feedback geven</t>
   </si>
   <si>
-    <t>Melding krijgen wanneer mijn pizza voorbereid is.</t>
-  </si>
-  <si>
     <t>feedback van andere klanten lezen</t>
   </si>
   <si>
     <t>Een overzicht van alle feedback</t>
   </si>
   <si>
-    <t>Klant bevestiging sturen wanneer de bestelling klaar is.</t>
-  </si>
-  <si>
-    <t>Een overzicht van de gemiddelde wachttijd van klanten</t>
-  </si>
-  <si>
     <t>Een overzicht van alle betalingen</t>
   </si>
   <si>
-    <t>Aangeven wanneer een bepaald topping niet meer op voorraad is</t>
-  </si>
-  <si>
-    <t>Een reminder wanneer de 90 minuten bijna zijn verstreken</t>
-  </si>
-  <si>
     <t>Keuze tussen glutenvrij of verschillende tarwe</t>
   </si>
   <si>
@@ -157,9 +136,6 @@
     <t>Een overzicht van mijn bestelling</t>
   </si>
   <si>
-    <t>Keukenvoorraad bijbestellen</t>
-  </si>
-  <si>
     <t>Een statistiek van alle inkomsten en uitgaven.</t>
   </si>
   <si>
@@ -172,41 +148,26 @@
     <t>Totaal</t>
   </si>
   <si>
-    <t>De prijzen beheren</t>
-  </si>
-  <si>
     <t>een filter functie</t>
   </si>
   <si>
-    <t>Beneden 2 tabjes</t>
-  </si>
-  <si>
-    <t>prijzen per 100 gram toppings / per pizzabodem</t>
-  </si>
-  <si>
     <t>grafiek instellen</t>
   </si>
   <si>
-    <t>Notificatie</t>
-  </si>
-  <si>
     <t>1 tot 5 sterren en beoordeling</t>
   </si>
   <si>
-    <t>Aangeven of ik langer blijf dan 90 minuten</t>
-  </si>
-  <si>
-    <t>Could have</t>
-  </si>
-  <si>
     <t>per betaalmethode</t>
+  </si>
+  <si>
+    <t>een nagerecht bestellen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -221,14 +182,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,12 +202,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -266,16 +215,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,13 +233,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,11 +549,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,17 +583,17 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -665,7 +607,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -674,12 +616,12 @@
         <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -693,7 +635,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -705,12 +647,12 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -722,12 +664,12 @@
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
@@ -736,12 +678,12 @@
         <v>30</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -750,12 +692,12 @@
         <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
@@ -769,7 +711,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -783,10 +725,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>30</v>
@@ -795,15 +737,15 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>30</v>
@@ -814,69 +756,69 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C14">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
       <c r="C15">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>60</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C18">
         <v>60</v>
@@ -884,65 +826,33 @@
       <c r="D18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E18" t="s">
-        <v>39</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19">
         <v>60</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C20">
-        <v>60</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21">
-        <v>60</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22">
-        <f>C3+C4+C5+C6+C7+C8+C9+C10+C11+C12+C13+C14+C15+C16+C17+C18+C19+C20+C21</f>
-        <v>730</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>48</v>
-      </c>
+        <f>C3+C4+C5+C6+C7+C8+C9+C10+C11+C12+C14+C15+C16+C17+C18+C19</f>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -953,11 +863,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,335 +897,203 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="6">
         <v>60</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6">
         <v>30</v>
       </c>
-      <c r="C4" s="7">
+      <c r="D4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6">
         <v>30</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="D5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="B6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="6">
+        <v>60</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6">
+        <v>80</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6">
         <v>30</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="7">
-        <v>20</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="7">
-        <v>60</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="7">
-        <v>80</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>50</v>
-      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="7">
-        <v>50</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>49</v>
-      </c>
+      <c r="A9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5">
+        <f>+C3+C4+C5+C6+C7+C8</f>
+        <v>290</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="7">
-        <v>20</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="6"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" s="7">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="7">
-        <v>50</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="6"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="7">
-        <v>20</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="7">
-        <v>30</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="9">
-        <v>40</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="8"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6">
-        <f>+C4+C3+C5+C6+C7+C8+C9+C10+C11+C12+C13+C14+C15+C16+C17+C18</f>
-        <v>520</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>